<commit_message>
experimenting with training values
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,13 +449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>285.8479309082031</v>
+        <v>72.04933929443359</v>
       </c>
       <c r="C2" t="n">
-        <v>282.756220636854</v>
+        <v>85.54615384615384</v>
       </c>
       <c r="D2" t="n">
-        <v>3.091710271349086</v>
+        <v>13.49681455172025</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>116.8584365844727</v>
+        <v>24.95390892028809</v>
       </c>
       <c r="C3" t="n">
-        <v>99.75445058317986</v>
+        <v>24.65333333333334</v>
       </c>
       <c r="D3" t="n">
-        <v>17.1039860012928</v>
+        <v>0.30057558695475</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2523.1337890625</v>
+        <v>40.07955169677734</v>
       </c>
       <c r="C4" t="n">
-        <v>1808.569838619922</v>
+        <v>74.82307692307693</v>
       </c>
       <c r="D4" t="n">
-        <v>714.5639504425778</v>
+        <v>34.74352522629958</v>
       </c>
     </row>
     <row r="5">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>144.4116973876953</v>
+        <v>6.885591506958008</v>
       </c>
       <c r="C5" t="n">
-        <v>147.3859099070129</v>
+        <v>3.188461538461539</v>
       </c>
       <c r="D5" t="n">
-        <v>2.974212519317547</v>
+        <v>3.697129968496469</v>
       </c>
     </row>
     <row r="6">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>511.0298461914062</v>
+        <v>57.96519470214844</v>
       </c>
       <c r="C6" t="n">
-        <v>621.0586661570801</v>
+        <v>53.96153846153846</v>
       </c>
       <c r="D6" t="n">
-        <v>110.0288199656738</v>
+        <v>4.003656240609978</v>
       </c>
     </row>
     <row r="7">
@@ -519,265 +519,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2536.42529296875</v>
+        <v>56.00526809692383</v>
       </c>
       <c r="C7" t="n">
-        <v>3484.320557491289</v>
+        <v>54.17692307692307</v>
       </c>
       <c r="D7" t="n">
-        <v>947.8952645225395</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>179.0279235839844</v>
-      </c>
-      <c r="C8" t="n">
-        <v>248.015873015873</v>
-      </c>
-      <c r="D8" t="n">
-        <v>68.98794943188864</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>132.2456207275391</v>
-      </c>
-      <c r="C9" t="n">
-        <v>144.9695563931574</v>
-      </c>
-      <c r="D9" t="n">
-        <v>12.72393566561837</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>80.95379638671875</v>
-      </c>
-      <c r="C10" t="n">
-        <v>71.57013873596124</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9.383657650757513</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>229.3900146484375</v>
-      </c>
-      <c r="C11" t="n">
-        <v>218.4916791085539</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10.89833553988356</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>240.8892059326172</v>
-      </c>
-      <c r="C12" t="n">
-        <v>169.5969246424332</v>
-      </c>
-      <c r="D12" t="n">
-        <v>71.29228129018404</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>195.2693939208984</v>
-      </c>
-      <c r="C13" t="n">
-        <v>126.8045259461568</v>
-      </c>
-      <c r="D13" t="n">
-        <v>68.46486797474159</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>117.9057998657227</v>
-      </c>
-      <c r="C14" t="n">
-        <v>119.3835467766442</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.477746910921567</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2526.6953125</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2333.094041636755</v>
-      </c>
-      <c r="D15" t="n">
-        <v>193.6012708632447</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>306.4122924804688</v>
-      </c>
-      <c r="C16" t="n">
-        <v>302.2144073850211</v>
-      </c>
-      <c r="D16" t="n">
-        <v>4.197885095447646</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>509.1178894042969</v>
-      </c>
-      <c r="C17" t="n">
-        <v>229.0345313601128</v>
-      </c>
-      <c r="D17" t="n">
-        <v>280.0833580441841</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>28.57252311706543</v>
-      </c>
-      <c r="C18" t="n">
-        <v>70.96392667060911</v>
-      </c>
-      <c r="D18" t="n">
-        <v>42.39140355354368</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>97.69632720947266</v>
-      </c>
-      <c r="C19" t="n">
-        <v>67.22515254938463</v>
-      </c>
-      <c r="D19" t="n">
-        <v>30.47117466008802</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>194.8542022705078</v>
-      </c>
-      <c r="C20" t="n">
-        <v>376.702405099971</v>
-      </c>
-      <c r="D20" t="n">
-        <v>181.8482028294632</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>120.2388076782227</v>
-      </c>
-      <c r="C21" t="n">
-        <v>262.6050420168067</v>
-      </c>
-      <c r="D21" t="n">
-        <v>142.3662343385841</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>236.6900329589844</v>
-      </c>
-      <c r="C22" t="n">
-        <v>63.04558680892337</v>
-      </c>
-      <c r="D22" t="n">
-        <v>173.644446150061</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>508.7684936523438</v>
-      </c>
-      <c r="C23" t="n">
-        <v>592.2551252847381</v>
-      </c>
-      <c r="D23" t="n">
-        <v>83.48663163239439</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2530.919921875</v>
-      </c>
-      <c r="C24" t="n">
-        <v>2646.579804560261</v>
-      </c>
-      <c r="D24" t="n">
-        <v>115.6598826852605</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>-61.59263610839844</v>
-      </c>
-      <c r="C25" t="n">
-        <v>138.1626493219402</v>
-      </c>
-      <c r="D25" t="n">
-        <v>199.7552854303386</v>
+        <v>1.828345020000754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>